<commit_message>
updates files - Nov. 22
</commit_message>
<xml_diff>
--- a/screening_deep_new.xlsx
+++ b/screening_deep_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ΔΗΜΗΤΡΗΣ\Documents\GitHubs\AI-marine-litter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF98ABF2-812C-4FD9-83EE-63E094D59300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E22D18-9C3B-4C41-ABB0-5608669E6AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29670" yWindow="285" windowWidth="26340" windowHeight="14100" xr2:uid="{9E4A43DE-8FF9-4A91-B492-0B4C1599A160}"/>
+    <workbookView xWindow="29310" yWindow="675" windowWidth="25845" windowHeight="14850" xr2:uid="{9E4A43DE-8FF9-4A91-B492-0B4C1599A160}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2065,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789D46A0-4CC3-42C0-9023-C48815470A65}">
   <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2132,6 +2132,9 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
       <c r="B2" s="18" t="s">
         <v>243</v>
       </c>
@@ -2173,6 +2176,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
       <c r="B3" s="18" t="s">
         <v>244</v>
       </c>
@@ -2212,6 +2218,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
       <c r="B4" s="18" t="s">
         <v>245</v>
       </c>
@@ -2253,6 +2262,9 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>245</v>
       </c>
@@ -2294,7 +2306,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="72"/>
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
       <c r="B6" s="72" t="s">
         <v>298</v>
       </c>
@@ -2336,7 +2350,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
       <c r="B7" s="4" t="s">
         <v>246</v>
       </c>
@@ -2376,6 +2392,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
       <c r="B8" s="18" t="s">
         <v>247</v>
       </c>
@@ -2415,7 +2434,9 @@
       <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" s="90" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18"/>
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
       <c r="B9" s="18" t="s">
         <v>248</v>
       </c>
@@ -2457,7 +2478,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" s="90" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="72"/>
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
       <c r="B10" s="72" t="s">
         <v>348</v>
       </c>
@@ -2499,7 +2522,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" s="90" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="72"/>
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
       <c r="B11" s="72" t="s">
         <v>291</v>
       </c>
@@ -2539,7 +2564,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" s="90" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>249</v>
       </c>
@@ -2581,7 +2608,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="18">
+        <v>12</v>
+      </c>
       <c r="B13" s="4" t="s">
         <v>249</v>
       </c>
@@ -2623,7 +2652,9 @@
       </c>
     </row>
     <row r="14" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="18">
+        <v>13</v>
+      </c>
       <c r="B14" s="4" t="s">
         <v>249</v>
       </c>
@@ -2665,7 +2696,9 @@
       </c>
     </row>
     <row r="15" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
       <c r="B15" s="4" t="s">
         <v>249</v>
       </c>
@@ -2707,7 +2740,9 @@
       </c>
     </row>
     <row r="16" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="72"/>
+      <c r="A16" s="18">
+        <v>15</v>
+      </c>
       <c r="B16" s="72" t="s">
         <v>337</v>
       </c>
@@ -2747,7 +2782,9 @@
       </c>
     </row>
     <row r="17" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="72"/>
+      <c r="A17" s="18">
+        <v>16</v>
+      </c>
       <c r="B17" s="72" t="s">
         <v>332</v>
       </c>
@@ -2789,7 +2826,9 @@
       </c>
     </row>
     <row r="18" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="72"/>
+      <c r="A18" s="18">
+        <v>17</v>
+      </c>
       <c r="B18" s="72" t="s">
         <v>312</v>
       </c>
@@ -2827,6 +2866,9 @@
       </c>
     </row>
     <row r="19" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18">
+        <v>18</v>
+      </c>
       <c r="B19" s="18" t="s">
         <v>250</v>
       </c>
@@ -2866,7 +2908,9 @@
       </c>
     </row>
     <row r="20" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="72"/>
+      <c r="A20" s="18">
+        <v>19</v>
+      </c>
       <c r="B20" s="72" t="s">
         <v>355</v>
       </c>
@@ -2908,7 +2952,9 @@
       </c>
     </row>
     <row r="21" spans="1:14" s="91" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="72"/>
+      <c r="A21" s="18">
+        <v>20</v>
+      </c>
       <c r="B21" s="72" t="s">
         <v>351</v>
       </c>
@@ -2950,6 +2996,9 @@
       </c>
     </row>
     <row r="22" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="18">
+        <v>21</v>
+      </c>
       <c r="B22" s="18" t="s">
         <v>251</v>
       </c>
@@ -2991,6 +3040,9 @@
       </c>
     </row>
     <row r="23" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="18">
+        <v>22</v>
+      </c>
       <c r="B23" s="18" t="s">
         <v>252</v>
       </c>
@@ -3030,7 +3082,9 @@
       </c>
     </row>
     <row r="24" spans="1:14" s="72" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="18"/>
+      <c r="A24" s="18">
+        <v>23</v>
+      </c>
       <c r="B24" s="18" t="s">
         <v>253</v>
       </c>
@@ -3072,6 +3126,9 @@
       </c>
     </row>
     <row r="25" spans="1:14" s="18" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="18">
+        <v>24</v>
+      </c>
       <c r="B25" s="18" t="s">
         <v>254</v>
       </c>
@@ -3113,6 +3170,9 @@
       </c>
     </row>
     <row r="26" spans="1:14" s="72" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="18">
+        <v>25</v>
+      </c>
       <c r="B26" s="72" t="s">
         <v>327</v>
       </c>
@@ -3152,7 +3212,9 @@
       <c r="N26" s="73"/>
     </row>
     <row r="27" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="72"/>
+      <c r="A27" s="18">
+        <v>26</v>
+      </c>
       <c r="B27" s="72" t="s">
         <v>299</v>
       </c>
@@ -3194,6 +3256,9 @@
       </c>
     </row>
     <row r="28" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="18">
+        <v>27</v>
+      </c>
       <c r="B28" s="18" t="s">
         <v>255</v>
       </c>
@@ -3235,7 +3300,9 @@
       </c>
     </row>
     <row r="29" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
+      <c r="A29" s="18">
+        <v>28</v>
+      </c>
       <c r="B29" s="18" t="s">
         <v>256</v>
       </c>
@@ -3275,7 +3342,9 @@
       </c>
     </row>
     <row r="30" spans="1:14" s="72" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
+      <c r="A30" s="18">
+        <v>29</v>
+      </c>
       <c r="B30" s="18" t="s">
         <v>257</v>
       </c>
@@ -3317,7 +3386,9 @@
       </c>
     </row>
     <row r="31" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="72"/>
+      <c r="A31" s="18">
+        <v>30</v>
+      </c>
       <c r="B31" s="72" t="s">
         <v>359</v>
       </c>
@@ -3359,7 +3430,9 @@
       </c>
     </row>
     <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="18"/>
+      <c r="A32" s="18">
+        <v>31</v>
+      </c>
       <c r="B32" s="18" t="s">
         <v>258</v>
       </c>
@@ -3401,7 +3474,9 @@
       </c>
     </row>
     <row r="33" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
+      <c r="A33" s="18">
+        <v>32</v>
+      </c>
       <c r="B33" s="18" t="s">
         <v>259</v>
       </c>
@@ -3443,7 +3518,9 @@
       </c>
     </row>
     <row r="34" spans="1:14" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="18"/>
+      <c r="A34" s="18">
+        <v>33</v>
+      </c>
       <c r="B34" s="18" t="s">
         <v>259</v>
       </c>
@@ -3485,6 +3562,9 @@
       </c>
     </row>
     <row r="35" spans="1:14" s="72" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="18">
+        <v>34</v>
+      </c>
       <c r="B35" s="72" t="s">
         <v>259</v>
       </c>
@@ -3526,7 +3606,9 @@
       </c>
     </row>
     <row r="36" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="18"/>
+      <c r="A36" s="18">
+        <v>35</v>
+      </c>
       <c r="B36" s="18" t="s">
         <v>260</v>
       </c>
@@ -3568,6 +3650,9 @@
       </c>
     </row>
     <row r="37" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="18">
+        <v>36</v>
+      </c>
       <c r="B37" s="72" t="s">
         <v>416</v>
       </c>
@@ -3607,6 +3692,9 @@
       </c>
     </row>
     <row r="38" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="18">
+        <v>37</v>
+      </c>
       <c r="B38" s="18" t="s">
         <v>417</v>
       </c>
@@ -3646,6 +3734,9 @@
       </c>
     </row>
     <row r="39" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="18">
+        <v>38</v>
+      </c>
       <c r="B39" s="18" t="s">
         <v>263</v>
       </c>
@@ -3685,7 +3776,9 @@
       <c r="N39" s="19"/>
     </row>
     <row r="40" spans="1:14" s="89" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="72"/>
+      <c r="A40" s="18">
+        <v>39</v>
+      </c>
       <c r="B40" s="72" t="s">
         <v>406</v>
       </c>
@@ -3727,7 +3820,9 @@
       </c>
     </row>
     <row r="41" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="4"/>
+      <c r="A41" s="18">
+        <v>40</v>
+      </c>
       <c r="B41" s="4" t="s">
         <v>264</v>
       </c>
@@ -3769,7 +3864,9 @@
       </c>
     </row>
     <row r="42" spans="1:14" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="72"/>
+      <c r="A42" s="18">
+        <v>41</v>
+      </c>
       <c r="B42" s="72" t="s">
         <v>265</v>
       </c>
@@ -3807,6 +3904,9 @@
       <c r="N42" s="73"/>
     </row>
     <row r="43" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="18">
+        <v>42</v>
+      </c>
       <c r="B43" s="72" t="s">
         <v>400</v>
       </c>
@@ -3848,7 +3948,9 @@
       </c>
     </row>
     <row r="44" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="18"/>
+      <c r="A44" s="18">
+        <v>43</v>
+      </c>
       <c r="B44" s="18" t="s">
         <v>266</v>
       </c>
@@ -3890,7 +3992,9 @@
       </c>
     </row>
     <row r="45" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
+      <c r="A45" s="18">
+        <v>44</v>
+      </c>
       <c r="B45" s="4" t="s">
         <v>267</v>
       </c>
@@ -3930,6 +4034,9 @@
       </c>
     </row>
     <row r="46" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="18">
+        <v>45</v>
+      </c>
       <c r="B46" s="4" t="s">
         <v>268</v>
       </c>
@@ -3967,7 +4074,9 @@
       </c>
     </row>
     <row r="47" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
+      <c r="A47" s="18">
+        <v>46</v>
+      </c>
       <c r="B47" s="4" t="s">
         <v>269</v>
       </c>
@@ -4005,7 +4114,9 @@
       </c>
     </row>
     <row r="48" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="18"/>
+      <c r="A48" s="18">
+        <v>47</v>
+      </c>
       <c r="B48" s="18" t="s">
         <v>341</v>
       </c>
@@ -4047,7 +4158,9 @@
       </c>
     </row>
     <row r="49" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="72"/>
+      <c r="A49" s="18">
+        <v>48</v>
+      </c>
       <c r="B49" s="72" t="s">
         <v>270</v>
       </c>
@@ -4087,7 +4200,9 @@
       </c>
     </row>
     <row r="50" spans="1:14" s="87" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="72"/>
+      <c r="A50" s="18">
+        <v>49</v>
+      </c>
       <c r="B50" s="72" t="s">
         <v>271</v>
       </c>
@@ -4129,7 +4244,9 @@
       </c>
     </row>
     <row r="51" spans="1:14" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="72"/>
+      <c r="A51" s="18">
+        <v>50</v>
+      </c>
       <c r="B51" s="72" t="s">
         <v>272</v>
       </c>
@@ -4167,7 +4284,9 @@
       </c>
     </row>
     <row r="52" spans="1:14" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="72"/>
+      <c r="A52" s="18">
+        <v>51</v>
+      </c>
       <c r="B52" s="72" t="s">
         <v>315</v>
       </c>
@@ -4201,7 +4320,9 @@
       <c r="N52" s="73"/>
     </row>
     <row r="53" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
+      <c r="A53" s="18">
+        <v>52</v>
+      </c>
       <c r="B53" s="18" t="s">
         <v>273</v>
       </c>
@@ -4239,7 +4360,9 @@
       </c>
     </row>
     <row r="54" spans="1:14" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="18"/>
+      <c r="A54" s="18">
+        <v>53</v>
+      </c>
       <c r="B54" s="18" t="s">
         <v>274</v>
       </c>
@@ -4281,7 +4404,9 @@
       </c>
     </row>
     <row r="55" spans="1:14" s="77" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="72"/>
+      <c r="A55" s="18">
+        <v>54</v>
+      </c>
       <c r="B55" s="72" t="s">
         <v>275</v>
       </c>
@@ -4323,7 +4448,9 @@
       </c>
     </row>
     <row r="56" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="18"/>
+      <c r="A56" s="18">
+        <v>55</v>
+      </c>
       <c r="B56" s="18" t="s">
         <v>276</v>
       </c>
@@ -4363,7 +4490,9 @@
       <c r="N56" s="19"/>
     </row>
     <row r="57" spans="1:14" s="71" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="72"/>
+      <c r="A57" s="18">
+        <v>56</v>
+      </c>
       <c r="B57" s="72" t="s">
         <v>293</v>
       </c>
@@ -4405,7 +4534,9 @@
       </c>
     </row>
     <row r="58" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="72"/>
+      <c r="A58" s="18">
+        <v>57</v>
+      </c>
       <c r="B58" s="72" t="s">
         <v>305</v>
       </c>
@@ -4443,7 +4574,9 @@
       </c>
     </row>
     <row r="59" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="72"/>
+      <c r="A59" s="18">
+        <v>58</v>
+      </c>
       <c r="B59" s="72" t="s">
         <v>410</v>
       </c>
@@ -4485,7 +4618,9 @@
       </c>
     </row>
     <row r="60" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
+      <c r="A60" s="18">
+        <v>59</v>
+      </c>
       <c r="B60" s="4" t="s">
         <v>277</v>
       </c>
@@ -4523,7 +4658,9 @@
       </c>
     </row>
     <row r="61" spans="1:14" s="70" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="72"/>
+      <c r="A61" s="18">
+        <v>60</v>
+      </c>
       <c r="B61" s="72" t="s">
         <v>301</v>
       </c>
@@ -4565,7 +4702,9 @@
       </c>
     </row>
     <row r="62" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="72"/>
+      <c r="A62" s="18">
+        <v>61</v>
+      </c>
       <c r="B62" s="72" t="s">
         <v>278</v>
       </c>
@@ -4603,7 +4742,9 @@
       </c>
     </row>
     <row r="63" spans="1:14" s="71" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="72"/>
+      <c r="A63" s="18">
+        <v>62</v>
+      </c>
       <c r="B63" s="72" t="s">
         <v>279</v>
       </c>
@@ -4645,7 +4786,9 @@
       </c>
     </row>
     <row r="64" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="72"/>
+      <c r="A64" s="18">
+        <v>63</v>
+      </c>
       <c r="B64" s="72" t="s">
         <v>280</v>
       </c>
@@ -4687,7 +4830,9 @@
       </c>
     </row>
     <row r="65" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="4"/>
+      <c r="A65" s="18">
+        <v>64</v>
+      </c>
       <c r="B65" s="4" t="s">
         <v>281</v>
       </c>
@@ -4729,7 +4874,9 @@
       </c>
     </row>
     <row r="66" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="72"/>
+      <c r="A66" s="18">
+        <v>65</v>
+      </c>
       <c r="B66" s="72" t="s">
         <v>323</v>
       </c>
@@ -4767,7 +4914,9 @@
       </c>
     </row>
     <row r="67" spans="1:14" s="78" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="72"/>
+      <c r="A67" s="18">
+        <v>66</v>
+      </c>
       <c r="B67" s="72" t="s">
         <v>222</v>
       </c>
@@ -4809,7 +4958,9 @@
       </c>
     </row>
     <row r="68" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="72"/>
+      <c r="A68" s="18">
+        <v>67</v>
+      </c>
       <c r="B68" s="72" t="s">
         <v>292</v>
       </c>
@@ -4847,7 +4998,9 @@
       </c>
     </row>
     <row r="69" spans="1:14" s="70" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="72"/>
+      <c r="A69" s="18">
+        <v>68</v>
+      </c>
       <c r="B69" s="72" t="s">
         <v>295</v>
       </c>
@@ -4889,7 +5042,9 @@
       </c>
     </row>
     <row r="70" spans="1:14" s="71" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="72"/>
+      <c r="A70" s="18">
+        <v>69</v>
+      </c>
       <c r="B70" s="72" t="s">
         <v>295</v>
       </c>
@@ -4931,7 +5086,9 @@
       </c>
     </row>
     <row r="71" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="72"/>
+      <c r="A71" s="18">
+        <v>70</v>
+      </c>
       <c r="B71" s="72" t="s">
         <v>333</v>
       </c>
@@ -4973,7 +5130,9 @@
       </c>
     </row>
     <row r="72" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="72"/>
+      <c r="A72" s="18">
+        <v>71</v>
+      </c>
       <c r="B72" s="72" t="s">
         <v>296</v>
       </c>
@@ -5015,7 +5174,9 @@
       </c>
     </row>
     <row r="73" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="72"/>
+      <c r="A73" s="18">
+        <v>72</v>
+      </c>
       <c r="B73" s="72" t="s">
         <v>398</v>
       </c>
@@ -5057,7 +5218,9 @@
       </c>
     </row>
     <row r="74" spans="1:14" s="71" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="72"/>
+      <c r="A74" s="18">
+        <v>73</v>
+      </c>
       <c r="B74" s="72" t="s">
         <v>282</v>
       </c>
@@ -5099,7 +5262,9 @@
       </c>
     </row>
     <row r="75" spans="1:14" s="71" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="72"/>
+      <c r="A75" s="18">
+        <v>74</v>
+      </c>
       <c r="B75" s="72" t="s">
         <v>297</v>
       </c>
@@ -5141,7 +5306,9 @@
       </c>
     </row>
     <row r="76" spans="1:14" s="70" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="72"/>
+      <c r="A76" s="18">
+        <v>75</v>
+      </c>
       <c r="B76" s="72" t="s">
         <v>283</v>
       </c>
@@ -5183,7 +5350,9 @@
       </c>
     </row>
     <row r="77" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="4"/>
+      <c r="A77" s="18">
+        <v>76</v>
+      </c>
       <c r="B77" s="4" t="s">
         <v>365</v>
       </c>
@@ -5223,7 +5392,9 @@
       </c>
     </row>
     <row r="78" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="72"/>
+      <c r="A78" s="18">
+        <v>77</v>
+      </c>
       <c r="B78" s="72" t="s">
         <v>294</v>
       </c>
@@ -5261,7 +5432,9 @@
       </c>
     </row>
     <row r="79" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="18"/>
+      <c r="A79" s="18">
+        <v>78</v>
+      </c>
       <c r="B79" s="18" t="s">
         <v>284</v>
       </c>
@@ -5301,7 +5474,9 @@
       </c>
     </row>
     <row r="80" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="18"/>
+      <c r="A80" s="18">
+        <v>79</v>
+      </c>
       <c r="B80" s="18" t="s">
         <v>285</v>
       </c>
@@ -5341,7 +5516,9 @@
       </c>
     </row>
     <row r="81" spans="1:14" s="92" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="72"/>
+      <c r="A81" s="18">
+        <v>80</v>
+      </c>
       <c r="B81" s="72" t="s">
         <v>286</v>
       </c>
@@ -5383,7 +5560,9 @@
       </c>
     </row>
     <row r="82" spans="1:14" s="78" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="72"/>
+      <c r="A82" s="18">
+        <v>81</v>
+      </c>
       <c r="B82" s="72" t="s">
         <v>287</v>
       </c>
@@ -5425,7 +5604,9 @@
       </c>
     </row>
     <row r="83" spans="1:14" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="86"/>
+      <c r="A83" s="18">
+        <v>82</v>
+      </c>
       <c r="B83" s="86" t="s">
         <v>288</v>
       </c>
@@ -5467,7 +5648,9 @@
       </c>
     </row>
     <row r="84" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="83"/>
+      <c r="A84" s="18">
+        <v>83</v>
+      </c>
       <c r="B84" s="83" t="s">
         <v>289</v>
       </c>
@@ -5509,7 +5692,9 @@
       </c>
     </row>
     <row r="85" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="83"/>
+      <c r="A85" s="18">
+        <v>84</v>
+      </c>
       <c r="B85" s="83" t="s">
         <v>290</v>
       </c>
@@ -5547,7 +5732,9 @@
       </c>
     </row>
     <row r="86" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="83"/>
+      <c r="A86" s="18">
+        <v>85</v>
+      </c>
       <c r="B86" s="83" t="s">
         <v>290</v>
       </c>

</xml_diff>